<commit_message>
added mainForm(simple) and navigation from login
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -75,6 +75,18 @@
   </x:si>
   <x:si>
     <x:t>6765</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Elizaveta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lizavainer</x:t>
+  </x:si>
+  <x:si>
+    <x:t>tester</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -526,6 +538,22 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:2">
+      <x:c r="A14" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Added mainForm and mainTeacher. functionality not yet added
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -87,6 +87,9 @@
   </x:si>
   <x:si>
     <x:t>test</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
   </x:si>
 </x:sst>
 </file>
@@ -554,6 +557,14 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
+    <x:row r="15" spans="1:2">
+      <x:c r="A15" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
unit test and Design
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -56,6 +56,24 @@
   </x:si>
   <x:si>
     <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>zechaad</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1234%z</x:t>
+  </x:si>
+  <x:si>
+    <x:t>xds</x:t>
+  </x:si>
+  <x:si>
+    <x:t>34562</x:t>
+  </x:si>
+  <x:si>
+    <x:t>zechariah</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1234</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -484,6 +502,30 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
commiting so i can pull properly 22_05
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -56,6 +56,18 @@
   </x:si>
   <x:si>
     <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>testliz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
+  </x:si>
+  <x:si>
+    <x:t>testproft</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test1</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -484,6 +496,30 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:2">
+      <x:c r="A11" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:2">
+      <x:c r="A12" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
added ui ux to login signup+animations,a little glitchy but works 24_05
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -80,6 +80,9 @@
   </x:si>
   <x:si>
     <x:t>33</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
   </x:si>
 </x:sst>
 </file>
@@ -556,6 +559,14 @@
         <x:v>21</x:v>
       </x:c>
     </x:row>
+    <x:row r="16" spans="1:2">
+      <x:c r="A16" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Designing a question editing page
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -82,7 +82,7 @@
     <x:t>33</x:t>
   </x:si>
   <x:si>
-    <x:t/>
+    <x:t>zecha</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -564,7 +564,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>19</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added "taz", mail and changes to database
"taz" and mail are now requirements for signup
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -20,69 +20,6 @@
   </x:si>
   <x:si>
     <x:t>Password</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Hello</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ds</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dsd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sdsds</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sdssd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dddd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>ddd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dfddfdfd</x:t>
-  </x:si>
-  <x:si>
-    <x:t>dfdff</x:t>
-  </x:si>
-  <x:si>
-    <x:t>עעעעעעעע</x:t>
-  </x:si>
-  <x:si>
-    <x:t>עעעעעע</x:t>
-  </x:si>
-  <x:si>
-    <x:t>11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>testliz</x:t>
-  </x:si>
-  <x:si>
-    <x:t>test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>testproft</x:t>
-  </x:si>
-  <x:si>
-    <x:t>test1</x:t>
-  </x:si>
-  <x:si>
-    <x:t>zechariah</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1234</x:t>
-  </x:si>
-  <x:si>
-    <x:t>22</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33</x:t>
-  </x:si>
-  <x:si>
-    <x:t>zecha</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -447,126 +384,6 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2">
-      <x:c r="A2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="B2" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:2">
-      <x:c r="A3" s="0" t="s">
-        <x:v>3</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>4</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:2">
-      <x:c r="A4" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>6</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:2">
-      <x:c r="A5" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:2">
-      <x:c r="A6" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="B6" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:2">
-      <x:c r="A7" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B7" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:2">
-      <x:c r="A8" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B8" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:2">
-      <x:c r="A9" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-      <x:c r="B9" s="0" t="s">
-        <x:v>13</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:2">
-      <x:c r="A10" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="B10" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:2">
-      <x:c r="A11" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="B11" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:2">
-      <x:c r="A12" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="B12" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:2">
-      <x:c r="A13" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="B13" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:2">
-      <x:c r="A14" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="B14" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:2">
-      <x:c r="A15" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="B15" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:2">
-      <x:c r="A16" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="B16" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Added designes,will continue tmr. 26_05
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -20,6 +20,42 @@
   </x:si>
   <x:si>
     <x:t>Password</x:t>
+  </x:si>
+  <x:si>
+    <x:t>testA11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>testA11,11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AAAA1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AAAAAAAA1,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nathan</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Andgame1!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>lizTest</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LizTest1!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LizTest2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LizTest2!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LizTester</x:t>
+  </x:si>
+  <x:si>
+    <x:t>LizTest3!</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -384,6 +420,54 @@
         <x:v>1</x:v>
       </x:c>
     </x:row>
+    <x:row r="2" spans="1:2">
+      <x:c r="A2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:2">
+      <x:c r="A3" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:2">
+      <x:c r="A4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:2">
+      <x:c r="A5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:2">
+      <x:c r="A6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:2">
+      <x:c r="A7" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Added password feature and signup
1. Icon for show password or hide password in login and signup.
2. When you sign up automatically moves to next stage, no need to login again.
3.Clear input when you move to login or signup.
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -56,6 +56,18 @@
   </x:si>
   <x:si>
     <x:t>LizTest3!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ShonJob1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test1!!!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Habuf</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Habuf12!</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -468,6 +480,22 @@
         <x:v>13</x:v>
       </x:c>
     </x:row>
+    <x:row r="8" spans="1:2">
+      <x:c r="A8" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:2">
+      <x:c r="A9" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
added difficulty in test
added difficulty in test to database and remove insert name after test
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -68,6 +68,12 @@
   </x:si>
   <x:si>
     <x:t>Habuf12!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aviv12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>aviv123!</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -496,6 +502,14 @@
         <x:v>17</x:v>
       </x:c>
     </x:row>
+    <x:row r="10" spans="1:2">
+      <x:c r="A10" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Added 30 unit tests to LoginSignup
Added 30 unit tests to LoginSignup.
All of them work and they all pass.
</commit_message>
<xml_diff>
--- a/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
+++ b/WinFormsApp1/WinFormsApp1/bin/Debug/net8.0-windows/Info.xlsx
@@ -86,6 +86,12 @@
   </x:si>
   <x:si>
     <x:t>David2929,</x:t>
+  </x:si>
+  <x:si>
+    <x:t>DeezNutz</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TestJob1!</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -538,6 +544,14 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
+    <x:row r="13" spans="1:2">
+      <x:c r="A13" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>